<commit_message>
Added 'price' to components and finished the arrays view.
</commit_message>
<xml_diff>
--- a/ExcelFiles/photoComponents.xlsx
+++ b/ExcelFiles/photoComponents.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jose-\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jose-\Desktop\Programming\CSharp\SolstatProjectUI\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="106">
   <si>
     <t>Paneles</t>
   </si>
@@ -339,6 +339,9 @@
   </si>
   <si>
     <t>YY Solar Co., Ltd.</t>
+  </si>
+  <si>
+    <t>Precio</t>
   </si>
 </sst>
 </file>
@@ -754,10 +757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G114"/>
+  <dimension ref="A1:H114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -771,7 +774,7 @@
     <col min="7" max="7" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -793,8 +796,11 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -816,8 +822,11 @@
       <c r="G2" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -839,8 +848,11 @@
       <c r="G3" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -862,8 +874,11 @@
       <c r="G4" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -885,8 +900,11 @@
       <c r="G5" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -908,8 +926,11 @@
       <c r="G6" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -931,8 +952,11 @@
       <c r="G7" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -954,8 +978,11 @@
       <c r="G8" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -977,8 +1004,11 @@
       <c r="G9" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1000,8 +1030,11 @@
       <c r="G10" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -1023,8 +1056,11 @@
       <c r="G11" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
@@ -1046,8 +1082,11 @@
       <c r="G12" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -1069,8 +1108,11 @@
       <c r="G13" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1092,8 +1134,11 @@
       <c r="G14" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1115,8 +1160,11 @@
       <c r="G15" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1138,8 +1186,11 @@
       <c r="G16" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -1161,8 +1212,11 @@
       <c r="G17" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -1184,8 +1238,11 @@
       <c r="G18" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -1207,8 +1264,11 @@
       <c r="G19" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -1230,8 +1290,11 @@
       <c r="G20" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
@@ -1253,8 +1316,11 @@
       <c r="G21" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>15</v>
       </c>
@@ -1276,8 +1342,11 @@
       <c r="G22" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>15</v>
       </c>
@@ -1299,8 +1368,11 @@
       <c r="G23" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>15</v>
       </c>
@@ -1322,8 +1394,11 @@
       <c r="G24" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>15</v>
       </c>
@@ -1345,8 +1420,11 @@
       <c r="G25" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>15</v>
       </c>
@@ -1368,8 +1446,11 @@
       <c r="G26" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>15</v>
       </c>
@@ -1391,8 +1472,11 @@
       <c r="G27" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>16</v>
       </c>
@@ -1414,8 +1498,11 @@
       <c r="G28" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>16</v>
       </c>
@@ -1437,8 +1524,11 @@
       <c r="G29" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>16</v>
       </c>
@@ -1460,8 +1550,11 @@
       <c r="G30" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>16</v>
       </c>
@@ -1483,8 +1576,11 @@
       <c r="G31" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>16</v>
       </c>
@@ -1506,8 +1602,11 @@
       <c r="G32" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>22</v>
       </c>
@@ -1529,8 +1628,11 @@
       <c r="G33" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>22</v>
       </c>
@@ -1552,8 +1654,11 @@
       <c r="G34" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>22</v>
       </c>
@@ -1575,8 +1680,11 @@
       <c r="G35" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>22</v>
       </c>
@@ -1598,8 +1706,11 @@
       <c r="G36" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>27</v>
       </c>
@@ -1621,8 +1732,11 @@
       <c r="G37" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>27</v>
       </c>
@@ -1644,8 +1758,11 @@
       <c r="G38" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>27</v>
       </c>
@@ -1667,8 +1784,11 @@
       <c r="G39" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>27</v>
       </c>
@@ -1690,8 +1810,11 @@
       <c r="G40" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>32</v>
       </c>
@@ -1713,8 +1836,11 @@
       <c r="G41" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>32</v>
       </c>
@@ -1736,8 +1862,11 @@
       <c r="G42" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>32</v>
       </c>
@@ -1759,8 +1888,11 @@
       <c r="G43" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>32</v>
       </c>
@@ -1782,8 +1914,11 @@
       <c r="G44" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>32</v>
       </c>
@@ -1805,8 +1940,11 @@
       <c r="G45" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>38</v>
       </c>
@@ -1828,8 +1966,11 @@
       <c r="G46" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>38</v>
       </c>
@@ -1851,8 +1992,11 @@
       <c r="G47" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>38</v>
       </c>
@@ -1874,8 +2018,11 @@
       <c r="G48" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>38</v>
       </c>
@@ -1897,8 +2044,11 @@
       <c r="G49" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>38</v>
       </c>
@@ -1920,8 +2070,11 @@
       <c r="G50" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>44</v>
       </c>
@@ -1943,8 +2096,11 @@
       <c r="G51" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>44</v>
       </c>
@@ -1966,8 +2122,11 @@
       <c r="G52" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>44</v>
       </c>
@@ -1989,8 +2148,11 @@
       <c r="G53" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>44</v>
       </c>
@@ -2012,8 +2174,11 @@
       <c r="G54" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>44</v>
       </c>
@@ -2035,8 +2200,11 @@
       <c r="G55" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>50</v>
       </c>
@@ -2058,8 +2226,11 @@
       <c r="G56" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>50</v>
       </c>
@@ -2081,8 +2252,11 @@
       <c r="G57" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>50</v>
       </c>
@@ -2104,8 +2278,11 @@
       <c r="G58" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>50</v>
       </c>
@@ -2127,8 +2304,11 @@
       <c r="G59" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H59">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>50</v>
       </c>
@@ -2150,8 +2330,11 @@
       <c r="G60" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H60">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>56</v>
       </c>
@@ -2173,8 +2356,11 @@
       <c r="G61" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>56</v>
       </c>
@@ -2196,8 +2382,11 @@
       <c r="G62" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>56</v>
       </c>
@@ -2219,8 +2408,11 @@
       <c r="G63" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>56</v>
       </c>
@@ -2242,8 +2434,11 @@
       <c r="G64" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H64">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>56</v>
       </c>
@@ -2265,8 +2460,11 @@
       <c r="G65" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H65">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>62</v>
       </c>
@@ -2288,8 +2486,11 @@
       <c r="G66" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H66">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>62</v>
       </c>
@@ -2311,8 +2512,11 @@
       <c r="G67" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H67">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>62</v>
       </c>
@@ -2334,8 +2538,11 @@
       <c r="G68" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H68">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>62</v>
       </c>
@@ -2357,8 +2564,11 @@
       <c r="G69" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H69">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>62</v>
       </c>
@@ -2380,8 +2590,11 @@
       <c r="G70" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H70">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>62</v>
       </c>
@@ -2403,8 +2616,11 @@
       <c r="G71" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H71">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>62</v>
       </c>
@@ -2426,8 +2642,11 @@
       <c r="G72" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H72">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>70</v>
       </c>
@@ -2449,8 +2668,11 @@
       <c r="G73" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H73">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>70</v>
       </c>
@@ -2472,8 +2694,11 @@
       <c r="G74" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H74">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>70</v>
       </c>
@@ -2495,8 +2720,11 @@
       <c r="G75" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>70</v>
       </c>
@@ -2518,8 +2746,11 @@
       <c r="G76" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H76">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>70</v>
       </c>
@@ -2541,8 +2772,11 @@
       <c r="G77" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H77">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>70</v>
       </c>
@@ -2564,8 +2798,11 @@
       <c r="G78" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H78">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>70</v>
       </c>
@@ -2587,8 +2824,11 @@
       <c r="G79" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H79">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>70</v>
       </c>
@@ -2610,8 +2850,11 @@
       <c r="G80" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H80">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>78</v>
       </c>
@@ -2633,8 +2876,11 @@
       <c r="G81" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H81">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>78</v>
       </c>
@@ -2656,8 +2902,11 @@
       <c r="G82" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H82">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>78</v>
       </c>
@@ -2679,8 +2928,11 @@
       <c r="G83" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H83">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>78</v>
       </c>
@@ -2702,8 +2954,11 @@
       <c r="G84" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H84">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>83</v>
       </c>
@@ -2725,8 +2980,11 @@
       <c r="G85" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H85">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>83</v>
       </c>
@@ -2748,8 +3006,11 @@
       <c r="G86" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H86">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>83</v>
       </c>
@@ -2771,8 +3032,11 @@
       <c r="G87" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H87">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>83</v>
       </c>
@@ -2794,8 +3058,11 @@
       <c r="G88" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H88">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>83</v>
       </c>
@@ -2817,8 +3084,11 @@
       <c r="G89" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H89">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>83</v>
       </c>
@@ -2840,8 +3110,11 @@
       <c r="G90" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H90">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>83</v>
       </c>
@@ -2863,8 +3136,11 @@
       <c r="G91" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H91">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>91</v>
       </c>
@@ -2886,8 +3162,11 @@
       <c r="G92" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H92">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>91</v>
       </c>
@@ -2909,8 +3188,11 @@
       <c r="G93" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H93">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>91</v>
       </c>
@@ -2932,8 +3214,11 @@
       <c r="G94" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H94">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>91</v>
       </c>
@@ -2955,8 +3240,11 @@
       <c r="G95" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H95">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>91</v>
       </c>
@@ -2978,8 +3266,11 @@
       <c r="G96" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H96">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>92</v>
       </c>
@@ -3001,8 +3292,11 @@
       <c r="G97" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H97">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>92</v>
       </c>
@@ -3024,8 +3318,11 @@
       <c r="G98" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H98">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>92</v>
       </c>
@@ -3047,8 +3344,11 @@
       <c r="G99" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H99">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>92</v>
       </c>
@@ -3070,8 +3370,11 @@
       <c r="G100" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H100">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>92</v>
       </c>
@@ -3093,8 +3396,11 @@
       <c r="G101" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H101">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>98</v>
       </c>
@@ -3116,8 +3422,11 @@
       <c r="G102" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H102">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>98</v>
       </c>
@@ -3139,8 +3448,11 @@
       <c r="G103" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H103">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>98</v>
       </c>
@@ -3162,8 +3474,11 @@
       <c r="G104" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H104">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>98</v>
       </c>
@@ -3185,8 +3500,11 @@
       <c r="G105" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H105">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>98</v>
       </c>
@@ -3208,8 +3526,11 @@
       <c r="G106" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H106">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="6" t="s">
         <v>104</v>
       </c>
@@ -3231,8 +3552,11 @@
       <c r="G107" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H107">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="6" t="s">
         <v>104</v>
       </c>
@@ -3254,8 +3578,11 @@
       <c r="G108" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H108">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" s="6" t="s">
         <v>104</v>
       </c>
@@ -3277,8 +3604,11 @@
       <c r="G109" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H109">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" s="6" t="s">
         <v>104</v>
       </c>
@@ -3300,8 +3630,11 @@
       <c r="G110" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H110">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="6" t="s">
         <v>104</v>
       </c>
@@ -3323,8 +3656,11 @@
       <c r="G111" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H111">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="6" t="s">
         <v>104</v>
       </c>
@@ -3346,8 +3682,11 @@
       <c r="G112" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H112">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="6" t="s">
         <v>104</v>
       </c>
@@ -3369,8 +3708,11 @@
       <c r="G113" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H113">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="6" t="s">
         <v>104</v>
       </c>
@@ -3391,6 +3733,9 @@
       </c>
       <c r="G114" s="4" t="s">
         <v>12</v>
+      </c>
+      <c r="H114">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>